<commit_message>
Finetuning after sensor reassembly
</commit_message>
<xml_diff>
--- a/xls/rig-spring-preloader.xlsx
+++ b/xls/rig-spring-preloader.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\rig-bxt-spring-preloader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\rig-bxt-spring-preloader\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0936E0-2C57-45EF-98D1-9A69145581DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7511F8-2E49-4BB7-816E-DA316C55B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2D2A40A7-2858-4013-928A-A8FD95D1B3C1}"/>
   </bookViews>
@@ -194,9 +194,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>DESIRED STOP</t>
-  </si>
-  <si>
     <t>STATE = OPEN DOOR</t>
   </si>
   <si>
@@ -206,7 +203,10 @@
     <t>WAIT IN LOOP FOR USER TO OPEN DOOR</t>
   </si>
   <si>
-    <t xml:space="preserve"> LATEST STOP</t>
+    <t>DESIRED STOP AFTER SENSOR DETECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LATEST STOP AFTER START IF NO SENSOR DETECTION</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -534,26 +534,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -563,8 +545,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="10" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1055,13 +1054,13 @@
     </row>
     <row r="9" spans="7:17" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="8"/>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
       <c r="M9" s="12"/>
     </row>
     <row r="10" spans="7:17" x14ac:dyDescent="0.25">
@@ -1072,20 +1071,20 @@
         <v>11</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K10" s="16" t="s">
         <v>35</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="7:17" ht="30" x14ac:dyDescent="0.25">
       <c r="G11"/>
       <c r="I11"/>
-      <c r="J11" s="37" t="s">
-        <v>49</v>
+      <c r="J11" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>35</v>
@@ -1096,14 +1095,14 @@
     </row>
     <row r="12" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G12"/>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="15" t="s">
         <v>35</v>
@@ -1116,13 +1115,13 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="14" spans="7:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G15"/>
@@ -1210,13 +1209,13 @@
     </row>
     <row r="23" spans="7:13" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="8"/>
-      <c r="H23" s="34" t="s">
+      <c r="H23" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="7:13" x14ac:dyDescent="0.25">
@@ -1252,13 +1251,13 @@
     </row>
     <row r="27" spans="7:13" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="8"/>
-      <c r="H27" s="34" t="s">
+      <c r="H27" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
       <c r="M27" s="12"/>
     </row>
     <row r="28" spans="7:13" x14ac:dyDescent="0.25">
@@ -1319,7 +1318,7 @@
   <dimension ref="H10:N12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,19 +1327,19 @@
   </cols>
   <sheetData>
     <row r="10" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="40" t="s">
+      <c r="J10" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="34" t="s">
         <v>44</v>
       </c>
       <c r="N10" s="43" t="s">
@@ -1349,27 +1348,27 @@
     </row>
     <row r="11" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="39">
-        <v>7</v>
-      </c>
-      <c r="J11" s="39">
+        <v>49</v>
+      </c>
+      <c r="I11" s="33">
+        <v>4</v>
+      </c>
+      <c r="J11" s="33">
         <v>283</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="36">
         <f>I11+J11/360</f>
-        <v>7.7861111111111114</v>
-      </c>
-      <c r="L11" s="40">
+        <v>4.7861111111111114</v>
+      </c>
+      <c r="L11" s="34">
         <v>200</v>
       </c>
-      <c r="M11" s="40">
+      <c r="M11" s="34">
         <v>128</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="42">
         <f>K11*L11*M11</f>
-        <v>199324.44444444444</v>
+        <v>122524.44444444445</v>
       </c>
     </row>
     <row r="12" spans="8:14" x14ac:dyDescent="0.25">
@@ -1377,24 +1376,24 @@
         <v>50</v>
       </c>
       <c r="I12" s="31">
-        <v>8.3000000000000007</v>
+        <v>8</v>
       </c>
       <c r="J12" s="31">
-        <v>0</v>
-      </c>
-      <c r="K12" s="42">
+        <v>180</v>
+      </c>
+      <c r="K12" s="36">
         <f>I12+J12/360</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="L12" s="40">
+        <v>8.5</v>
+      </c>
+      <c r="L12" s="34">
         <v>200</v>
       </c>
-      <c r="M12" s="40">
+      <c r="M12" s="34">
         <v>128</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="42">
         <f>K12*L12*M12</f>
-        <v>212480.00000000003</v>
+        <v>217600</v>
       </c>
     </row>
   </sheetData>
@@ -1434,13 +1433,13 @@
       </c>
     </row>
     <row r="8" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
     </row>
     <row r="9" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
@@ -1525,13 +1524,13 @@
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
@@ -1559,13 +1558,13 @@
       </c>
     </row>
     <row r="22" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H22" s="36" t="s">
+      <c r="H22" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J23" t="s">

</xml_diff>

<commit_message>
Finetuning and naming "TWISTER"
</commit_message>
<xml_diff>
--- a/xls/rig-spring-preloader.xlsx
+++ b/xls/rig-spring-preloader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\rig-bxt-spring-preloader\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7511F8-2E49-4BB7-816E-DA316C55B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024E2BA2-A822-43A4-993F-E7416C040370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2D2A40A7-2858-4013-928A-A8FD95D1B3C1}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{2D2A40A7-2858-4013-928A-A8FD95D1B3C1}"/>
   </bookViews>
   <sheets>
     <sheet name="without feedback" sheetId="5" r:id="rId1"/>
@@ -545,6 +545,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="10" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -560,10 +563,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="9" fillId="10" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1054,13 +1054,13 @@
     </row>
     <row r="9" spans="7:17" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="8"/>
-      <c r="H9" s="37" t="s">
+      <c r="H9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
       <c r="M9" s="12"/>
     </row>
     <row r="10" spans="7:17" x14ac:dyDescent="0.25">
@@ -1115,13 +1115,13 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="14" spans="7:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="7:17" x14ac:dyDescent="0.25">
       <c r="G15"/>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="23" spans="7:13" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="8"/>
-      <c r="H23" s="39" t="s">
+      <c r="H23" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="7:13" x14ac:dyDescent="0.25">
@@ -1251,13 +1251,13 @@
     </row>
     <row r="27" spans="7:13" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="8"/>
-      <c r="H27" s="39" t="s">
+      <c r="H27" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
       <c r="M27" s="12"/>
     </row>
     <row r="28" spans="7:13" x14ac:dyDescent="0.25">
@@ -1318,7 +1318,7 @@
   <dimension ref="H10:N12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,7 +1342,7 @@
       <c r="M10" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="43" t="s">
+      <c r="N10" s="37" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1354,11 +1354,11 @@
         <v>4</v>
       </c>
       <c r="J11" s="33">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="K11" s="36">
         <f>I11+J11/360</f>
-        <v>4.7861111111111114</v>
+        <v>4.8166666666666664</v>
       </c>
       <c r="L11" s="34">
         <v>200</v>
@@ -1366,9 +1366,9 @@
       <c r="M11" s="34">
         <v>128</v>
       </c>
-      <c r="N11" s="42">
+      <c r="N11" s="43">
         <f>K11*L11*M11</f>
-        <v>122524.44444444445</v>
+        <v>123306.66666666666</v>
       </c>
     </row>
     <row r="12" spans="8:14" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
       <c r="M12" s="34">
         <v>128</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="43">
         <f>K12*L12*M12</f>
         <v>217600</v>
       </c>
@@ -1433,13 +1433,13 @@
       </c>
     </row>
     <row r="8" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
     </row>
     <row r="9" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
@@ -1524,13 +1524,13 @@
       </c>
     </row>
     <row r="18" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H18" s="41" t="s">
+      <c r="H18" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
@@ -1558,13 +1558,13 @@
       </c>
     </row>
     <row r="22" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J23" t="s">

</xml_diff>